<commit_message>
Updated date parsing and scan counters
</commit_message>
<xml_diff>
--- a/tests/out1.xlsx
+++ b/tests/out1.xlsx
@@ -3153,7 +3153,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>http://190.160.53.126/cPzGZqbbrF2WtX/5aWaSd/XAWyg/AF8g1pcudGHa/5Tu4GPZZYIHhX7XZ5b7/</t>
+          <t>http://190.160.53.126/L3uZ0FJkzd00V/PnEJQO9BTZTIH75sat/</t>
         </is>
       </c>
       <c r="H2" t="n">
@@ -3164,7 +3164,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>2022-05-31 00:34:14</t>
+          <t>2022-05-31 11:20:33</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -3212,18 +3212,18 @@
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr">
         <is>
-          <t>http://190.160.53.126/</t>
+          <t>http://190.160.53.126/cPzGZqbbrF2WtX/5aWaSd/XAWyg/AF8g1pcudGHa/5Tu4GPZZYIHhX7XZ5b7/</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="I3" t="n">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>2022-05-30 07:08:35</t>
+          <t>2022-05-31 00:34:14</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -3271,18 +3271,18 @@
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr">
         <is>
-          <t>http://190.160.53.126/L3uZ0FJkzd00V/PnEJQO9BTZTIH75sat/</t>
+          <t>http://190.160.53.126/</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="I4" t="n">
         <v>93</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>2022-05-29 20:11:46</t>
+          <t>2022-05-30 07:08:35</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -9592,7 +9592,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9618,25 +9618,30 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>detected_urls_positives</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>detected_urls_total</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>detected_urls_scan_date</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Engine</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Engine_detected</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Engine_result</t>
         </is>
@@ -9659,24 +9664,27 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>100</v>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>1653984678</t>
-        </is>
+        <v>4</v>
+      </c>
+      <c r="E2" t="n">
+        <v>86</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
+          <t>2022-05-31 10:11:18</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
           <t>Comodo Valkyrie Verdict</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>Comodo Valkyrie Verdict</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>suspicious</t>
         </is>
@@ -9699,24 +9707,27 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>100</v>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>1653984678</t>
-        </is>
+        <v>4</v>
+      </c>
+      <c r="E3" t="n">
+        <v>86</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
+          <t>2022-05-31 10:11:18</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
           <t>CRDF</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>CRDF</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>malicious</t>
         </is>
@@ -9739,24 +9750,27 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>100</v>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>1653984678</t>
-        </is>
+        <v>4</v>
+      </c>
+      <c r="E4" t="n">
+        <v>86</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
+          <t>2022-05-31 10:11:18</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
           <t>Fortinet</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="H4" t="inlineStr">
         <is>
           <t>Fortinet</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="I4" t="inlineStr">
         <is>
           <t>malware</t>
         </is>
@@ -9779,24 +9793,27 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>100</v>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>1653984678</t>
-        </is>
+        <v>4</v>
+      </c>
+      <c r="E5" t="n">
+        <v>86</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
+          <t>2022-05-31 10:11:18</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
           <t>AutoShun</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="H5" t="inlineStr">
         <is>
           <t>AutoShun</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="I5" t="inlineStr">
         <is>
           <t>malicious</t>
         </is>
@@ -9819,24 +9836,27 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>100</v>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>1653984678</t>
-        </is>
+        <v>4</v>
+      </c>
+      <c r="E6" t="n">
+        <v>86</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
+          <t>2022-05-31 10:11:18</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
           <t>Webroot</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
+      <c r="H6" t="inlineStr">
         <is>
           <t>Webroot</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
+      <c r="I6" t="inlineStr">
         <is>
           <t>malicious</t>
         </is>
@@ -9859,24 +9879,27 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>100</v>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>1653984678</t>
-        </is>
+        <v>4</v>
+      </c>
+      <c r="E7" t="n">
+        <v>86</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
+          <t>2022-05-31 10:11:18</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
           <t>Forcepoint ThreatSeeker</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="H7" t="inlineStr">
         <is>
           <t>Forcepoint ThreatSeeker</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
+      <c r="I7" t="inlineStr">
         <is>
           <t>suspicious</t>
         </is>

</xml_diff>

<commit_message>
updated documentation and directory mappings
</commit_message>
<xml_diff>
--- a/tests/out1.xlsx
+++ b/tests/out1.xlsx
@@ -9592,7 +9592,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:A2"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9600,10 +9600,308 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Field</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>detected_url</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>detected_urls_positives</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>detected_urls_total</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>detected_urls_scan_date</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Engine</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Engine_detected</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Engine_result</t>
+        </is>
+      </c>
+    </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Field</t>
+          <t>http://hecs.com</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>URL</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>http://hecs.com/</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>4</v>
+      </c>
+      <c r="E2" t="n">
+        <v>86</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2022-05-31 10:11:18</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Comodo Valkyrie Verdict</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Comodo Valkyrie Verdict</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>suspicious</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>http://hecs.com</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>URL</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>http://hecs.com/</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E3" t="n">
+        <v>86</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2022-05-31 10:11:18</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>CRDF</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>CRDF</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>malicious</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>http://hecs.com</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>URL</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>http://hecs.com/</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>4</v>
+      </c>
+      <c r="E4" t="n">
+        <v>86</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2022-05-31 10:11:18</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Fortinet</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Fortinet</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>malware</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>http://hecs.com</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>URL</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>http://hecs.com/</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>4</v>
+      </c>
+      <c r="E5" t="n">
+        <v>86</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2022-05-31 10:11:18</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>AutoShun</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>AutoShun</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>malicious</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>http://hecs.com</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>URL</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>http://hecs.com/</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>4</v>
+      </c>
+      <c r="E6" t="n">
+        <v>86</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2022-05-31 10:11:18</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Webroot</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Webroot</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>malicious</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>http://hecs.com</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>URL</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>http://hecs.com/</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>4</v>
+      </c>
+      <c r="E7" t="n">
+        <v>86</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2022-05-31 10:11:18</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Forcepoint ThreatSeeker</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Forcepoint ThreatSeeker</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>suspicious</t>
         </is>
       </c>
     </row>
@@ -9704,8 +10002,10 @@
           <t>Bkav</t>
         </is>
       </c>
-      <c r="D2" t="n">
-        <v>55</v>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -9760,8 +10060,10 @@
           <t>Lionic</t>
         </is>
       </c>
-      <c r="D3" t="n">
-        <v>55</v>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -9816,8 +10118,10 @@
           <t>Elastic</t>
         </is>
       </c>
-      <c r="D4" t="n">
-        <v>55</v>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -9872,8 +10176,10 @@
           <t>Cynet</t>
         </is>
       </c>
-      <c r="D5" t="n">
-        <v>55</v>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -9928,8 +10234,10 @@
           <t>McAfee</t>
         </is>
       </c>
-      <c r="D6" t="n">
-        <v>55</v>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -9984,8 +10292,10 @@
           <t>Malwarebytes</t>
         </is>
       </c>
-      <c r="D7" t="n">
-        <v>55</v>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -10040,8 +10350,10 @@
           <t>Sangfor</t>
         </is>
       </c>
-      <c r="D8" t="n">
-        <v>55</v>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -10096,8 +10408,10 @@
           <t>K7AntiVirus</t>
         </is>
       </c>
-      <c r="D9" t="n">
-        <v>55</v>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -10152,8 +10466,10 @@
           <t>BitDefender</t>
         </is>
       </c>
-      <c r="D10" t="n">
-        <v>55</v>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -10208,8 +10524,10 @@
           <t>K7GW</t>
         </is>
       </c>
-      <c r="D11" t="n">
-        <v>55</v>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -10264,8 +10582,10 @@
           <t>CrowdStrike</t>
         </is>
       </c>
-      <c r="D12" t="n">
-        <v>55</v>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -10320,8 +10640,10 @@
           <t>VirIT</t>
         </is>
       </c>
-      <c r="D13" t="n">
-        <v>55</v>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -10376,8 +10698,10 @@
           <t>Cyren</t>
         </is>
       </c>
-      <c r="D14" t="n">
-        <v>55</v>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -10432,8 +10756,10 @@
           <t>ESET-NOD32</t>
         </is>
       </c>
-      <c r="D15" t="n">
-        <v>55</v>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -10488,8 +10814,10 @@
           <t>APEX</t>
         </is>
       </c>
-      <c r="D16" t="n">
-        <v>55</v>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -10544,8 +10872,10 @@
           <t>Avast</t>
         </is>
       </c>
-      <c r="D17" t="n">
-        <v>55</v>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -10600,8 +10930,10 @@
           <t>ClamAV</t>
         </is>
       </c>
-      <c r="D18" t="n">
-        <v>55</v>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -10656,8 +10988,10 @@
           <t>Kaspersky</t>
         </is>
       </c>
-      <c r="D19" t="n">
-        <v>55</v>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -10712,8 +11046,10 @@
           <t>Alibaba</t>
         </is>
       </c>
-      <c r="D20" t="n">
-        <v>55</v>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -10768,8 +11104,10 @@
           <t>NANO-Antivirus</t>
         </is>
       </c>
-      <c r="D21" t="n">
-        <v>55</v>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -10824,8 +11162,10 @@
           <t>ViRobot</t>
         </is>
       </c>
-      <c r="D22" t="n">
-        <v>55</v>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -10880,8 +11220,10 @@
           <t>MicroWorld-eScan</t>
         </is>
       </c>
-      <c r="D23" t="n">
-        <v>55</v>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -10936,8 +11278,10 @@
           <t>Tencent</t>
         </is>
       </c>
-      <c r="D24" t="n">
-        <v>55</v>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -10992,8 +11336,10 @@
           <t>Ad-Aware</t>
         </is>
       </c>
-      <c r="D25" t="n">
-        <v>55</v>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -11048,8 +11394,10 @@
           <t>Emsisoft</t>
         </is>
       </c>
-      <c r="D26" t="n">
-        <v>55</v>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -11104,8 +11452,10 @@
           <t>Comodo</t>
         </is>
       </c>
-      <c r="D27" t="n">
-        <v>55</v>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -11160,8 +11510,10 @@
           <t>F-Secure</t>
         </is>
       </c>
-      <c r="D28" t="n">
-        <v>55</v>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -11216,8 +11568,10 @@
           <t>DrWeb</t>
         </is>
       </c>
-      <c r="D29" t="n">
-        <v>55</v>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -11272,8 +11626,10 @@
           <t>BitDefenderTheta</t>
         </is>
       </c>
-      <c r="D30" t="n">
-        <v>55</v>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -11328,8 +11684,10 @@
           <t>TrendMicro</t>
         </is>
       </c>
-      <c r="D31" t="n">
-        <v>55</v>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -11384,8 +11742,10 @@
           <t>McAfee-GW-Edition</t>
         </is>
       </c>
-      <c r="D32" t="n">
-        <v>55</v>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -11440,8 +11800,10 @@
           <t>Trapmine</t>
         </is>
       </c>
-      <c r="D33" t="n">
-        <v>55</v>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -11496,8 +11858,10 @@
           <t>FireEye</t>
         </is>
       </c>
-      <c r="D34" t="n">
-        <v>55</v>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -11552,8 +11916,10 @@
           <t>Sophos</t>
         </is>
       </c>
-      <c r="D35" t="n">
-        <v>55</v>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -11608,8 +11974,10 @@
           <t>Ikarus</t>
         </is>
       </c>
-      <c r="D36" t="n">
-        <v>55</v>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -11664,8 +12032,10 @@
           <t>Jiangmin</t>
         </is>
       </c>
-      <c r="D37" t="n">
-        <v>55</v>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -11720,8 +12090,10 @@
           <t>Webroot</t>
         </is>
       </c>
-      <c r="D38" t="n">
-        <v>55</v>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -11776,8 +12148,10 @@
           <t>Avira</t>
         </is>
       </c>
-      <c r="D39" t="n">
-        <v>55</v>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -11832,8 +12206,10 @@
           <t>Antiy-AVL</t>
         </is>
       </c>
-      <c r="D40" t="n">
-        <v>55</v>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -11888,8 +12264,10 @@
           <t>Microsoft</t>
         </is>
       </c>
-      <c r="D41" t="n">
-        <v>55</v>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -11944,8 +12322,10 @@
           <t>Arcabit</t>
         </is>
       </c>
-      <c r="D42" t="n">
-        <v>55</v>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -12000,8 +12380,10 @@
           <t>ZoneAlarm</t>
         </is>
       </c>
-      <c r="D43" t="n">
-        <v>55</v>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -12056,8 +12438,10 @@
           <t>GData</t>
         </is>
       </c>
-      <c r="D44" t="n">
-        <v>55</v>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -12112,8 +12496,10 @@
           <t>VBA32</t>
         </is>
       </c>
-      <c r="D45" t="n">
-        <v>55</v>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -12168,8 +12554,10 @@
           <t>ALYac</t>
         </is>
       </c>
-      <c r="D46" t="n">
-        <v>55</v>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -12224,8 +12612,10 @@
           <t>Cylance</t>
         </is>
       </c>
-      <c r="D47" t="n">
-        <v>55</v>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -12280,8 +12670,10 @@
           <t>TrendMicro-HouseCall</t>
         </is>
       </c>
-      <c r="D48" t="n">
-        <v>55</v>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -12336,8 +12728,10 @@
           <t>Rising</t>
         </is>
       </c>
-      <c r="D49" t="n">
-        <v>55</v>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -12392,8 +12786,10 @@
           <t>Yandex</t>
         </is>
       </c>
-      <c r="D50" t="n">
-        <v>55</v>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -12448,8 +12844,10 @@
           <t>SentinelOne</t>
         </is>
       </c>
-      <c r="D51" t="n">
-        <v>55</v>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -12504,8 +12902,10 @@
           <t>MaxSecure</t>
         </is>
       </c>
-      <c r="D52" t="n">
-        <v>55</v>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -12560,8 +12960,10 @@
           <t>Fortinet</t>
         </is>
       </c>
-      <c r="D53" t="n">
-        <v>55</v>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -12616,8 +13018,10 @@
           <t>AVG</t>
         </is>
       </c>
-      <c r="D54" t="n">
-        <v>55</v>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -12672,8 +13076,10 @@
           <t>Cybereason</t>
         </is>
       </c>
-      <c r="D55" t="n">
-        <v>55</v>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -12728,8 +13134,10 @@
           <t>Paloalto</t>
         </is>
       </c>
-      <c r="D56" t="n">
-        <v>55</v>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -12784,8 +13192,10 @@
           <t>Bkav</t>
         </is>
       </c>
-      <c r="D57" t="n">
-        <v>55</v>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -12840,8 +13250,10 @@
           <t>Lionic</t>
         </is>
       </c>
-      <c r="D58" t="n">
-        <v>55</v>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -12896,8 +13308,10 @@
           <t>Elastic</t>
         </is>
       </c>
-      <c r="D59" t="n">
-        <v>55</v>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -12952,8 +13366,10 @@
           <t>Cynet</t>
         </is>
       </c>
-      <c r="D60" t="n">
-        <v>55</v>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -13008,8 +13424,10 @@
           <t>McAfee</t>
         </is>
       </c>
-      <c r="D61" t="n">
-        <v>55</v>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -13064,8 +13482,10 @@
           <t>Malwarebytes</t>
         </is>
       </c>
-      <c r="D62" t="n">
-        <v>55</v>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -13120,8 +13540,10 @@
           <t>Sangfor</t>
         </is>
       </c>
-      <c r="D63" t="n">
-        <v>55</v>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -13176,8 +13598,10 @@
           <t>K7AntiVirus</t>
         </is>
       </c>
-      <c r="D64" t="n">
-        <v>55</v>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -13232,8 +13656,10 @@
           <t>BitDefender</t>
         </is>
       </c>
-      <c r="D65" t="n">
-        <v>55</v>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -13288,8 +13714,10 @@
           <t>K7GW</t>
         </is>
       </c>
-      <c r="D66" t="n">
-        <v>55</v>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -13344,8 +13772,10 @@
           <t>CrowdStrike</t>
         </is>
       </c>
-      <c r="D67" t="n">
-        <v>55</v>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -13400,8 +13830,10 @@
           <t>VirIT</t>
         </is>
       </c>
-      <c r="D68" t="n">
-        <v>55</v>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -13456,8 +13888,10 @@
           <t>Cyren</t>
         </is>
       </c>
-      <c r="D69" t="n">
-        <v>55</v>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -13512,8 +13946,10 @@
           <t>ESET-NOD32</t>
         </is>
       </c>
-      <c r="D70" t="n">
-        <v>55</v>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -13568,8 +14004,10 @@
           <t>APEX</t>
         </is>
       </c>
-      <c r="D71" t="n">
-        <v>55</v>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -13624,8 +14062,10 @@
           <t>Avast</t>
         </is>
       </c>
-      <c r="D72" t="n">
-        <v>55</v>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -13680,8 +14120,10 @@
           <t>ClamAV</t>
         </is>
       </c>
-      <c r="D73" t="n">
-        <v>55</v>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -13736,8 +14178,10 @@
           <t>Kaspersky</t>
         </is>
       </c>
-      <c r="D74" t="n">
-        <v>55</v>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -13792,8 +14236,10 @@
           <t>Alibaba</t>
         </is>
       </c>
-      <c r="D75" t="n">
-        <v>55</v>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -13848,8 +14294,10 @@
           <t>NANO-Antivirus</t>
         </is>
       </c>
-      <c r="D76" t="n">
-        <v>55</v>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -13904,8 +14352,10 @@
           <t>ViRobot</t>
         </is>
       </c>
-      <c r="D77" t="n">
-        <v>55</v>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -13960,8 +14410,10 @@
           <t>MicroWorld-eScan</t>
         </is>
       </c>
-      <c r="D78" t="n">
-        <v>55</v>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -14016,8 +14468,10 @@
           <t>Tencent</t>
         </is>
       </c>
-      <c r="D79" t="n">
-        <v>55</v>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -14072,8 +14526,10 @@
           <t>Ad-Aware</t>
         </is>
       </c>
-      <c r="D80" t="n">
-        <v>55</v>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -14128,8 +14584,10 @@
           <t>Emsisoft</t>
         </is>
       </c>
-      <c r="D81" t="n">
-        <v>55</v>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -14184,8 +14642,10 @@
           <t>Comodo</t>
         </is>
       </c>
-      <c r="D82" t="n">
-        <v>55</v>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
@@ -14240,8 +14700,10 @@
           <t>F-Secure</t>
         </is>
       </c>
-      <c r="D83" t="n">
-        <v>55</v>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -14296,8 +14758,10 @@
           <t>DrWeb</t>
         </is>
       </c>
-      <c r="D84" t="n">
-        <v>55</v>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -14352,8 +14816,10 @@
           <t>BitDefenderTheta</t>
         </is>
       </c>
-      <c r="D85" t="n">
-        <v>55</v>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -14408,8 +14874,10 @@
           <t>TrendMicro</t>
         </is>
       </c>
-      <c r="D86" t="n">
-        <v>55</v>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -14464,8 +14932,10 @@
           <t>McAfee-GW-Edition</t>
         </is>
       </c>
-      <c r="D87" t="n">
-        <v>55</v>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -14520,8 +14990,10 @@
           <t>Trapmine</t>
         </is>
       </c>
-      <c r="D88" t="n">
-        <v>55</v>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -14576,8 +15048,10 @@
           <t>FireEye</t>
         </is>
       </c>
-      <c r="D89" t="n">
-        <v>55</v>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -14632,8 +15106,10 @@
           <t>Sophos</t>
         </is>
       </c>
-      <c r="D90" t="n">
-        <v>55</v>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -14688,8 +15164,10 @@
           <t>Ikarus</t>
         </is>
       </c>
-      <c r="D91" t="n">
-        <v>55</v>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -14744,8 +15222,10 @@
           <t>Jiangmin</t>
         </is>
       </c>
-      <c r="D92" t="n">
-        <v>55</v>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -14800,8 +15280,10 @@
           <t>Webroot</t>
         </is>
       </c>
-      <c r="D93" t="n">
-        <v>55</v>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
@@ -14856,8 +15338,10 @@
           <t>Avira</t>
         </is>
       </c>
-      <c r="D94" t="n">
-        <v>55</v>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
@@ -14912,8 +15396,10 @@
           <t>Antiy-AVL</t>
         </is>
       </c>
-      <c r="D95" t="n">
-        <v>55</v>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -14968,8 +15454,10 @@
           <t>Microsoft</t>
         </is>
       </c>
-      <c r="D96" t="n">
-        <v>55</v>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -15024,8 +15512,10 @@
           <t>Arcabit</t>
         </is>
       </c>
-      <c r="D97" t="n">
-        <v>55</v>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
@@ -15080,8 +15570,10 @@
           <t>ZoneAlarm</t>
         </is>
       </c>
-      <c r="D98" t="n">
-        <v>55</v>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -15136,8 +15628,10 @@
           <t>GData</t>
         </is>
       </c>
-      <c r="D99" t="n">
-        <v>55</v>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -15192,8 +15686,10 @@
           <t>VBA32</t>
         </is>
       </c>
-      <c r="D100" t="n">
-        <v>55</v>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -15248,8 +15744,10 @@
           <t>ALYac</t>
         </is>
       </c>
-      <c r="D101" t="n">
-        <v>55</v>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -15304,8 +15802,10 @@
           <t>Cylance</t>
         </is>
       </c>
-      <c r="D102" t="n">
-        <v>55</v>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -15360,8 +15860,10 @@
           <t>TrendMicro-HouseCall</t>
         </is>
       </c>
-      <c r="D103" t="n">
-        <v>55</v>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -15416,8 +15918,10 @@
           <t>Rising</t>
         </is>
       </c>
-      <c r="D104" t="n">
-        <v>55</v>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -15472,8 +15976,10 @@
           <t>Yandex</t>
         </is>
       </c>
-      <c r="D105" t="n">
-        <v>55</v>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -15528,8 +16034,10 @@
           <t>SentinelOne</t>
         </is>
       </c>
-      <c r="D106" t="n">
-        <v>55</v>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -15584,8 +16092,10 @@
           <t>MaxSecure</t>
         </is>
       </c>
-      <c r="D107" t="n">
-        <v>55</v>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -15640,8 +16150,10 @@
           <t>Fortinet</t>
         </is>
       </c>
-      <c r="D108" t="n">
-        <v>55</v>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -15696,8 +16208,10 @@
           <t>AVG</t>
         </is>
       </c>
-      <c r="D109" t="n">
-        <v>55</v>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -15752,8 +16266,10 @@
           <t>Cybereason</t>
         </is>
       </c>
-      <c r="D110" t="n">
-        <v>55</v>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -15808,8 +16324,10 @@
           <t>Paloalto</t>
         </is>
       </c>
-      <c r="D111" t="n">
-        <v>55</v>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -15864,8 +16382,10 @@
           <t>Bkav</t>
         </is>
       </c>
-      <c r="D112" t="n">
-        <v>62</v>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -15920,8 +16440,10 @@
           <t>Elastic</t>
         </is>
       </c>
-      <c r="D113" t="n">
-        <v>62</v>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -15976,8 +16498,10 @@
           <t>MicroWorld-eScan</t>
         </is>
       </c>
-      <c r="D114" t="n">
-        <v>62</v>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -16032,8 +16556,10 @@
           <t>FireEye</t>
         </is>
       </c>
-      <c r="D115" t="n">
-        <v>62</v>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -16088,8 +16614,10 @@
           <t>CAT-QuickHeal</t>
         </is>
       </c>
-      <c r="D116" t="n">
-        <v>62</v>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
       <c r="E116" t="inlineStr">
         <is>
@@ -16144,8 +16672,10 @@
           <t>McAfee</t>
         </is>
       </c>
-      <c r="D117" t="n">
-        <v>62</v>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -16200,8 +16730,10 @@
           <t>Cylance</t>
         </is>
       </c>
-      <c r="D118" t="n">
-        <v>62</v>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -16256,8 +16788,10 @@
           <t>Zillya</t>
         </is>
       </c>
-      <c r="D119" t="n">
-        <v>62</v>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -16312,8 +16846,10 @@
           <t>Sangfor</t>
         </is>
       </c>
-      <c r="D120" t="n">
-        <v>62</v>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
       <c r="E120" t="inlineStr">
         <is>
@@ -16368,8 +16904,10 @@
           <t>CrowdStrike</t>
         </is>
       </c>
-      <c r="D121" t="n">
-        <v>62</v>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
       <c r="E121" t="inlineStr">
         <is>
@@ -16424,8 +16962,10 @@
           <t>K7GW</t>
         </is>
       </c>
-      <c r="D122" t="n">
-        <v>62</v>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -16480,8 +17020,10 @@
           <t>K7AntiVirus</t>
         </is>
       </c>
-      <c r="D123" t="n">
-        <v>62</v>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -16536,8 +17078,10 @@
           <t>Invincea</t>
         </is>
       </c>
-      <c r="D124" t="n">
-        <v>62</v>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -16592,8 +17136,10 @@
           <t>Baidu</t>
         </is>
       </c>
-      <c r="D125" t="n">
-        <v>62</v>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
       <c r="E125" t="inlineStr">
         <is>
@@ -16648,8 +17194,10 @@
           <t>Cyren</t>
         </is>
       </c>
-      <c r="D126" t="n">
-        <v>62</v>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
       <c r="E126" t="inlineStr">
         <is>
@@ -16704,8 +17252,10 @@
           <t>Symantec</t>
         </is>
       </c>
-      <c r="D127" t="n">
-        <v>62</v>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
       <c r="E127" t="inlineStr">
         <is>
@@ -16760,8 +17310,10 @@
           <t>TotalDefense</t>
         </is>
       </c>
-      <c r="D128" t="n">
-        <v>62</v>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -16816,8 +17368,10 @@
           <t>APEX</t>
         </is>
       </c>
-      <c r="D129" t="n">
-        <v>62</v>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -16872,8 +17426,10 @@
           <t>Avast</t>
         </is>
       </c>
-      <c r="D130" t="n">
-        <v>62</v>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -16928,8 +17484,10 @@
           <t>ClamAV</t>
         </is>
       </c>
-      <c r="D131" t="n">
-        <v>62</v>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -16984,8 +17542,10 @@
           <t>Kaspersky</t>
         </is>
       </c>
-      <c r="D132" t="n">
-        <v>62</v>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -17040,8 +17600,10 @@
           <t>BitDefender</t>
         </is>
       </c>
-      <c r="D133" t="n">
-        <v>62</v>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -17096,8 +17658,10 @@
           <t>NANO-Antivirus</t>
         </is>
       </c>
-      <c r="D134" t="n">
-        <v>62</v>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -17152,8 +17716,10 @@
           <t>Tencent</t>
         </is>
       </c>
-      <c r="D135" t="n">
-        <v>62</v>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -17208,8 +17774,10 @@
           <t>Ad-Aware</t>
         </is>
       </c>
-      <c r="D136" t="n">
-        <v>62</v>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -17264,8 +17832,10 @@
           <t>Emsisoft</t>
         </is>
       </c>
-      <c r="D137" t="n">
-        <v>62</v>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -17320,8 +17890,10 @@
           <t>Comodo</t>
         </is>
       </c>
-      <c r="D138" t="n">
-        <v>62</v>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -17376,8 +17948,10 @@
           <t>F-Secure</t>
         </is>
       </c>
-      <c r="D139" t="n">
-        <v>62</v>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
       <c r="E139" t="inlineStr">
         <is>
@@ -17432,8 +18006,10 @@
           <t>DrWeb</t>
         </is>
       </c>
-      <c r="D140" t="n">
-        <v>62</v>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -17488,8 +18064,10 @@
           <t>VIPRE</t>
         </is>
       </c>
-      <c r="D141" t="n">
-        <v>62</v>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -17544,8 +18122,10 @@
           <t>TrendMicro</t>
         </is>
       </c>
-      <c r="D142" t="n">
-        <v>62</v>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -17600,8 +18180,10 @@
           <t>McAfee-GW-Edition</t>
         </is>
       </c>
-      <c r="D143" t="n">
-        <v>62</v>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
       <c r="E143" t="inlineStr">
         <is>
@@ -17656,8 +18238,10 @@
           <t>Sophos</t>
         </is>
       </c>
-      <c r="D144" t="n">
-        <v>62</v>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
       <c r="E144" t="inlineStr">
         <is>
@@ -17712,8 +18296,10 @@
           <t>Ikarus</t>
         </is>
       </c>
-      <c r="D145" t="n">
-        <v>62</v>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
       <c r="E145" t="inlineStr">
         <is>
@@ -17768,8 +18354,10 @@
           <t>GData</t>
         </is>
       </c>
-      <c r="D146" t="n">
-        <v>62</v>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
       <c r="E146" t="inlineStr">
         <is>
@@ -17824,8 +18412,10 @@
           <t>Jiangmin</t>
         </is>
       </c>
-      <c r="D147" t="n">
-        <v>62</v>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -17880,8 +18470,10 @@
           <t>Webroot</t>
         </is>
       </c>
-      <c r="D148" t="n">
-        <v>62</v>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -17936,8 +18528,10 @@
           <t>Avira</t>
         </is>
       </c>
-      <c r="D149" t="n">
-        <v>62</v>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
       <c r="E149" t="inlineStr">
         <is>
@@ -17992,8 +18586,10 @@
           <t>Antiy-AVL</t>
         </is>
       </c>
-      <c r="D150" t="n">
-        <v>62</v>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
       <c r="E150" t="inlineStr">
         <is>
@@ -18048,8 +18644,10 @@
           <t>Arcabit</t>
         </is>
       </c>
-      <c r="D151" t="n">
-        <v>62</v>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -18104,8 +18702,10 @@
           <t>ViRobot</t>
         </is>
       </c>
-      <c r="D152" t="n">
-        <v>62</v>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -18160,8 +18760,10 @@
           <t>ZoneAlarm</t>
         </is>
       </c>
-      <c r="D153" t="n">
-        <v>62</v>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -18216,8 +18818,10 @@
           <t>Microsoft</t>
         </is>
       </c>
-      <c r="D154" t="n">
-        <v>62</v>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -18272,8 +18876,10 @@
           <t>Cynet</t>
         </is>
       </c>
-      <c r="D155" t="n">
-        <v>62</v>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
       <c r="E155" t="inlineStr">
         <is>
@@ -18328,8 +18934,10 @@
           <t>AhnLab-V3</t>
         </is>
       </c>
-      <c r="D156" t="n">
-        <v>62</v>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
       <c r="E156" t="inlineStr">
         <is>
@@ -18384,8 +18992,10 @@
           <t>Acronis</t>
         </is>
       </c>
-      <c r="D157" t="n">
-        <v>62</v>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
       <c r="E157" t="inlineStr">
         <is>
@@ -18440,8 +19050,10 @@
           <t>BitDefenderTheta</t>
         </is>
       </c>
-      <c r="D158" t="n">
-        <v>62</v>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
       <c r="E158" t="inlineStr">
         <is>
@@ -18496,8 +19108,10 @@
           <t>ALYac</t>
         </is>
       </c>
-      <c r="D159" t="n">
-        <v>62</v>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
       <c r="E159" t="inlineStr">
         <is>
@@ -18552,8 +19166,10 @@
           <t>MAX</t>
         </is>
       </c>
-      <c r="D160" t="n">
-        <v>62</v>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -18608,8 +19224,10 @@
           <t>VBA32</t>
         </is>
       </c>
-      <c r="D161" t="n">
-        <v>62</v>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -18664,8 +19282,10 @@
           <t>Malwarebytes</t>
         </is>
       </c>
-      <c r="D162" t="n">
-        <v>62</v>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -18720,8 +19340,10 @@
           <t>ESET-NOD32</t>
         </is>
       </c>
-      <c r="D163" t="n">
-        <v>62</v>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
       <c r="E163" t="inlineStr">
         <is>
@@ -18776,8 +19398,10 @@
           <t>TrendMicro-HouseCall</t>
         </is>
       </c>
-      <c r="D164" t="n">
-        <v>62</v>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
       <c r="E164" t="inlineStr">
         <is>
@@ -18832,8 +19456,10 @@
           <t>Rising</t>
         </is>
       </c>
-      <c r="D165" t="n">
-        <v>62</v>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -18888,8 +19514,10 @@
           <t>Yandex</t>
         </is>
       </c>
-      <c r="D166" t="n">
-        <v>62</v>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
       <c r="E166" t="inlineStr">
         <is>
@@ -18944,8 +19572,10 @@
           <t>SentinelOne</t>
         </is>
       </c>
-      <c r="D167" t="n">
-        <v>62</v>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -19000,8 +19630,10 @@
           <t>eGambit</t>
         </is>
       </c>
-      <c r="D168" t="n">
-        <v>62</v>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
       <c r="E168" t="inlineStr"/>
       <c r="F168" t="inlineStr">
@@ -19052,8 +19684,10 @@
           <t>Fortinet</t>
         </is>
       </c>
-      <c r="D169" t="n">
-        <v>62</v>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -19108,8 +19742,10 @@
           <t>AVG</t>
         </is>
       </c>
-      <c r="D170" t="n">
-        <v>62</v>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -19164,8 +19800,10 @@
           <t>Cybereason</t>
         </is>
       </c>
-      <c r="D171" t="n">
-        <v>62</v>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -19220,8 +19858,10 @@
           <t>Panda</t>
         </is>
       </c>
-      <c r="D172" t="n">
-        <v>62</v>
+      <c r="D172" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
       <c r="E172" t="inlineStr">
         <is>
@@ -19276,8 +19916,10 @@
           <t>Qihoo-360</t>
         </is>
       </c>
-      <c r="D173" t="n">
-        <v>62</v>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
       </c>
       <c r="E173" t="inlineStr">
         <is>

</xml_diff>